<commit_message>
Minor modification of config for testing and testing files
</commit_message>
<xml_diff>
--- a/test_data/Roczny_2023.xlsx
+++ b/test_data/Roczny_2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dane\Python\Wlasne\Report\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A18520-9DC6-4056-B417-2689F5190480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E6569B8-B085-40E3-A76C-C2C761577EDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView showSheetTabs="0" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -996,18 +996,20 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1016,8 +1018,6 @@
     <xf numFmtId="2" fontId="0" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="95">
     <cellStyle name="20% — akcent 1 2" xfId="72" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
@@ -1456,7 +1456,7 @@
       <pane xSplit="1" ySplit="8" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="U3" sqref="U3"/>
+      <selection pane="bottomRight" activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1483,18 +1483,18 @@
       <c r="C1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="53" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="48"/>
-      <c r="F1" s="45"/>
+      <c r="F1" s="49"/>
       <c r="G1" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="51" t="s">
+      <c r="H1" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="45"/>
+      <c r="I1" s="49"/>
       <c r="J1" s="23" t="s">
         <v>6</v>
       </c>
@@ -1505,11 +1505,11 @@
         <v>8</v>
       </c>
       <c r="M1" s="48"/>
-      <c r="N1" s="45"/>
+      <c r="N1" s="49"/>
       <c r="O1" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="45"/>
+      <c r="P1" s="49"/>
       <c r="Q1" s="23" t="s">
         <v>10</v>
       </c>
@@ -1517,7 +1517,7 @@
         <v>11</v>
       </c>
       <c r="S1" s="48"/>
-      <c r="T1" s="45"/>
+      <c r="T1" s="49"/>
       <c r="U1" s="23" t="s">
         <v>12</v>
       </c>
@@ -1525,32 +1525,32 @@
         <v>13</v>
       </c>
       <c r="W1" s="48"/>
-      <c r="X1" s="45"/>
+      <c r="X1" s="49"/>
       <c r="Y1" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="Z1" s="45"/>
+      <c r="Z1" s="49"/>
     </row>
     <row r="2" spans="1:26" s="21" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="53"/>
+      <c r="A2" s="45"/>
       <c r="B2" s="20" t="s">
         <v>21</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="46" t="s">
+      <c r="D2" s="52" t="s">
         <v>22</v>
       </c>
       <c r="E2" s="48"/>
-      <c r="F2" s="45"/>
+      <c r="F2" s="49"/>
       <c r="G2" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="46" t="s">
+      <c r="H2" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="45"/>
+      <c r="I2" s="49"/>
       <c r="J2" s="18" t="s">
         <v>25</v>
       </c>
@@ -1561,11 +1561,11 @@
         <v>22</v>
       </c>
       <c r="M2" s="48"/>
-      <c r="N2" s="45"/>
+      <c r="N2" s="49"/>
       <c r="O2" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="P2" s="45"/>
+      <c r="P2" s="49"/>
       <c r="Q2" s="18" t="s">
         <v>21</v>
       </c>
@@ -1573,7 +1573,7 @@
         <v>22</v>
       </c>
       <c r="S2" s="48"/>
-      <c r="T2" s="45"/>
+      <c r="T2" s="49"/>
       <c r="U2" s="18" t="s">
         <v>27</v>
       </c>
@@ -1581,14 +1581,14 @@
         <v>22</v>
       </c>
       <c r="W2" s="48"/>
-      <c r="X2" s="45"/>
+      <c r="X2" s="49"/>
       <c r="Y2" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="Z2" s="45"/>
+      <c r="Z2" s="49"/>
     </row>
     <row r="3" spans="1:26" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="53"/>
+      <c r="A3" s="45"/>
       <c r="B3" s="19">
         <f>B4</f>
         <v>762.67000000000019</v>
@@ -1597,7 +1597,7 @@
         <f>C4</f>
         <v>368.42</v>
       </c>
-      <c r="D3" s="52">
+      <c r="D3" s="54">
         <f>+D4+F4+E4</f>
         <v>628.02</v>
       </c>
@@ -1607,11 +1607,11 @@
         <f>G4</f>
         <v>763.87999999999943</v>
       </c>
-      <c r="H3" s="47">
+      <c r="H3" s="51">
         <f>SUM(H4:I4)</f>
         <v>498.3599999999999</v>
       </c>
-      <c r="I3" s="45"/>
+      <c r="I3" s="49"/>
       <c r="J3" s="25">
         <f>J4</f>
         <v>500.64000000000016</v>
@@ -1620,45 +1620,45 @@
         <f>K4</f>
         <v>762.68000000000018</v>
       </c>
-      <c r="L3" s="49">
+      <c r="L3" s="47">
         <f>+L4+N4+M4</f>
         <v>628.02</v>
       </c>
       <c r="M3" s="48"/>
-      <c r="N3" s="45"/>
-      <c r="O3" s="49">
+      <c r="N3" s="49"/>
+      <c r="O3" s="47">
         <f>+O4+P4</f>
         <v>57.360000000000007</v>
       </c>
-      <c r="P3" s="45"/>
+      <c r="P3" s="49"/>
       <c r="Q3" s="25">
         <f>Q4</f>
         <v>763.87999999999943</v>
       </c>
-      <c r="R3" s="49">
+      <c r="R3" s="47">
         <f>+R4+T4+S4</f>
         <v>618.55000000000007</v>
       </c>
       <c r="S3" s="48"/>
-      <c r="T3" s="45"/>
+      <c r="T3" s="49"/>
       <c r="U3" s="25">
         <f>U4</f>
         <v>406.44000000000011</v>
       </c>
-      <c r="V3" s="49">
+      <c r="V3" s="47">
         <f>+V4+X4+W4</f>
         <v>618.55000000000007</v>
       </c>
       <c r="W3" s="48"/>
-      <c r="X3" s="45"/>
-      <c r="Y3" s="49">
+      <c r="X3" s="49"/>
+      <c r="Y3" s="47">
         <f>+Y4+Z4</f>
         <v>425.51000000000005</v>
       </c>
-      <c r="Z3" s="45"/>
+      <c r="Z3" s="49"/>
     </row>
     <row r="4" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="53"/>
+      <c r="A4" s="45"/>
       <c r="B4" s="40">
         <f t="shared" ref="B4:K4" si="0">SUM(B9:B736)</f>
         <v>762.67000000000019</v>
@@ -1761,7 +1761,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="54"/>
+      <c r="A5" s="46"/>
       <c r="B5" s="39" t="s">
         <v>15</v>
       </c>
@@ -9459,6 +9459,12 @@
   </sheetData>
   <autoFilter ref="A8:A396" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="22">
+    <mergeCell ref="Y3:Z3"/>
+    <mergeCell ref="R1:T1"/>
+    <mergeCell ref="V2:X2"/>
+    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="V1:X1"/>
     <mergeCell ref="A1:A5"/>
     <mergeCell ref="V3:X3"/>
     <mergeCell ref="L2:N2"/>
@@ -9473,13 +9479,7 @@
     <mergeCell ref="L1:N1"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="O1:P1"/>
-    <mergeCell ref="Y3:Z3"/>
-    <mergeCell ref="R1:T1"/>
-    <mergeCell ref="V2:X2"/>
-    <mergeCell ref="Y2:Z2"/>
-    <mergeCell ref="Y1:Z1"/>
     <mergeCell ref="O2:P2"/>
-    <mergeCell ref="V1:X1"/>
     <mergeCell ref="H1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="U1:V1 A1:E1 Y1 AA1:XFD1 O1 Q1:S1 G1:H1 J1:M1">

</xml_diff>